<commit_message>
Overwrite files from local
</commit_message>
<xml_diff>
--- a/scripts/parameters settings.xlsx
+++ b/scripts/parameters settings.xlsx
@@ -1610,10 +1610,10 @@
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
     <Closed_x0020_Date xmlns="9d238732-7262-4555-9fe6-01f908b108f7" xsi:nil="true"/>
-    <_dlc_DocId xmlns="9d238732-7262-4555-9fe6-01f908b108f7">S2557-345060206-30776</_dlc_DocId>
+    <_dlc_DocId xmlns="9d238732-7262-4555-9fe6-01f908b108f7">S2557-345060206-33722</_dlc_DocId>
     <_dlc_DocIdUrl xmlns="9d238732-7262-4555-9fe6-01f908b108f7">
-      <Url>https://nbncolimited.sharepoint.com/sites/S2557/_layouts/15/DocIdRedir.aspx?ID=S2557-345060206-30776</Url>
-      <Description>S2557-345060206-30776</Description>
+      <Url>https://nbncolimited.sharepoint.com/sites/S2557/_layouts/15/DocIdRedir.aspx?ID=S2557-345060206-33722</Url>
+      <Description>S2557-345060206-33722</Description>
     </_dlc_DocIdUrl>
   </documentManagement>
 </p:properties>

</xml_diff>